<commit_message>
create good card with js
</commit_message>
<xml_diff>
--- a/data/some_data.xlsx
+++ b/data/some_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\V-284\dev\alcomarket\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD5BB7C2-B2E0-4DB2-B641-813747C1069B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B65A5F-56F4-45F7-B5FD-A6821BFF8450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{696DC0A0-4D97-4E42-8A71-1E45AC4F62C5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>Водка</t>
   </si>
@@ -117,13 +117,148 @@
     <t>The Wine Group</t>
   </si>
   <si>
-    <t>Davide Campari-Milano S.p.A.</t>
-  </si>
-  <si>
-    <t>Gruppo Campari</t>
-  </si>
-  <si>
     <t>Heaven Hill Brands</t>
+  </si>
+  <si>
+    <t>Diageo была основана в 1997 году, когда Grand Metropolitan и Guinness объединились. Компания имеет корни, возводящиеся к началу 19 века, и владеет такими исторически важными брендами, как Johnnie Walker, Guinness и Smirnoff.</t>
+  </si>
+  <si>
+    <t>Pernod Ricard начал свою историю в 1805 году с создания абсента Pernod Fils во Франции. Компания стала международной силой, приобретая различные марки алкоголя, включая Chivas Regal, Absolut и Jameson.</t>
+  </si>
+  <si>
+    <t>Bacardi была основана в Кубе в 1862 году и остается семейной компанией. Она славится своим ромом, включая Bacardi Superior, и также производит другие алкогольные напитки.</t>
+  </si>
+  <si>
+    <t>Корни Moët Hennessy уходят в 1743 год, когда был создан Moët &amp; Chandon, один из известнейших производителей шампанского. Компания также известна своим коньяком Hennessy и роскошными напитками.</t>
+  </si>
+  <si>
+    <t>Brown-Forman начала свою историю в 1870 году с основания Jack Daniel's в Теннесси. Она также производит другие алкогольные напитки, такие как Finlandia Vodka и Woodford Reserve.</t>
+  </si>
+  <si>
+    <t>Beam Suntory объединила два исторических бренда - Jim Beam и Suntory. Jim Beam был основан в 1795 году, а Suntory - в 1899 году в Японии. Эта компания сочетает богатое наследие виски.</t>
+  </si>
+  <si>
+    <t>Constellation Brands начала как винодельческая компания в США в 1945 году и впоследствии приобрела множество марок пива, вина и текилы, включая Corona и Robert Mondavi.</t>
+  </si>
+  <si>
+    <t>Edrington Group была создана в 1860 году и специализируется на виски высокого качества, включая The Macallan и Highland Park.</t>
+  </si>
+  <si>
+    <t>William Grant &amp; Sons была основана в Шотландии в 1887 году и остается семейным предприятием. Она производит виски, такие как Glenfiddich и Balvenie.</t>
+  </si>
+  <si>
+    <t>Campari Group берет начало в Италии в 1860 году с создания Campari, известного аперитива. Компания также владеет другими известными брендами.</t>
+  </si>
+  <si>
+    <t>Remy Cointreau начала свою историю более двух веков назад во Франции и специализируется на премиум-ликерах и коньяке, включая Remy Martin и Cointreau.</t>
+  </si>
+  <si>
+    <t>Sazerac Company - это американская компания, с историей, которая насчитывает более 150 лет. Она производит различные алкогольные напитки, включая Buffalo Trace Bourbon и Southern Comfort.</t>
+  </si>
+  <si>
+    <t>The Wine Group начала свою историю в 1981 году и стала одним из крупнейших производителей вина в США, владея марками, такими как Franzia и Cupcake.</t>
+  </si>
+  <si>
+    <t>Heaven Hill Brands - это американская компания, которая начала свою историю в 1935 году и специализируется на производстве виски и других алкогольных напитков, включая Evan Williams и Elijah Craig.</t>
+  </si>
+  <si>
+    <t>diageo</t>
+  </si>
+  <si>
+    <t>pernod-ricard</t>
+  </si>
+  <si>
+    <t>bacardi-limited</t>
+  </si>
+  <si>
+    <t>moet-hennessy</t>
+  </si>
+  <si>
+    <t>brown-forman</t>
+  </si>
+  <si>
+    <t>beam-suntory</t>
+  </si>
+  <si>
+    <t>constellation-brands</t>
+  </si>
+  <si>
+    <t>edrington-group</t>
+  </si>
+  <si>
+    <t>william-grant-sons</t>
+  </si>
+  <si>
+    <t>campari-group</t>
+  </si>
+  <si>
+    <t>remy-cointreau</t>
+  </si>
+  <si>
+    <t>sazerac</t>
+  </si>
+  <si>
+    <t>wine-group</t>
+  </si>
+  <si>
+    <t>heaven-hill-brands</t>
+  </si>
+  <si>
+    <t>vodka</t>
+  </si>
+  <si>
+    <t>rum</t>
+  </si>
+  <si>
+    <t>whisky</t>
+  </si>
+  <si>
+    <t>tequila</t>
+  </si>
+  <si>
+    <t>brandy</t>
+  </si>
+  <si>
+    <t>gin</t>
+  </si>
+  <si>
+    <t>vermouth</t>
+  </si>
+  <si>
+    <t>cognac</t>
+  </si>
+  <si>
+    <t>champagne</t>
+  </si>
+  <si>
+    <t>beer</t>
+  </si>
+  <si>
+    <t>wine</t>
+  </si>
+  <si>
+    <t>liqueur</t>
+  </si>
+  <si>
+    <t>absinthe</t>
+  </si>
+  <si>
+    <t>mezcal</t>
+  </si>
+  <si>
+    <t>Игристое вино</t>
+  </si>
+  <si>
+    <t>sparkling_wine</t>
+  </si>
+  <si>
+    <t>The Macallan</t>
+  </si>
+  <si>
+    <t>Шотландский бренд виски из региона Хайленд.</t>
+  </si>
+  <si>
+    <t>macallan</t>
   </si>
 </sst>
 </file>
@@ -476,141 +611,276 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353EADFF-F8CD-44B5-96B7-A0617D27E916}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" t="s">
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" t="s">
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="C13" t="s">
+      <c r="B13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="C14" t="s">
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>29</v>
+      <c r="E14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>